<commit_message>
Actualización de tipos de datos de algunas variables
</commit_message>
<xml_diff>
--- a/DisenoBD/Diseño_BD.xlsx
+++ b/DisenoBD/Diseño_BD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\OneDrive - Universidad Fidélitas\1_Ingeniería Sistemas\22_Programacion_Avanzada_Web\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4B952F-2C45-40CC-8888-3A80AEF61EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66CF34A-3A47-48F6-83B8-FDC0F61E73B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22635" yWindow="1320" windowWidth="17280" windowHeight="8970" xr2:uid="{CE70A62E-34E2-4F22-8578-7B258473A79B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CE70A62E-34E2-4F22-8578-7B258473A79B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="44">
   <si>
     <t>Tipo</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>varchar(200)</t>
-  </si>
-  <si>
-    <t>bigint</t>
   </si>
   <si>
     <t>Tipo_Usuario</t>
@@ -175,7 +172,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,6 +184,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -298,24 +302,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -634,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6BF18F-7FBC-4503-A33D-E0AD7A1C3ED1}">
   <dimension ref="D2:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -653,42 +659,42 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6"/>
-      <c r="H2" s="3" t="s">
+      <c r="E2" s="8"/>
+      <c r="F2" s="9"/>
+      <c r="H2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="L2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+    </row>
+    <row r="3" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="L2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-    </row>
-    <row r="3" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8" t="s">
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8" t="s">
+      <c r="H3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="L3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8" t="s">
+      <c r="L3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4" t="s">
         <v>0</v>
       </c>
     </row>
@@ -697,25 +703,25 @@
         <v>3</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>2</v>
@@ -734,14 +740,14 @@
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="4:14" x14ac:dyDescent="0.3">
@@ -753,7 +759,7 @@
         <v>4</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
@@ -769,17 +775,17 @@
         <v>4</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
+        <v>25</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
     </row>
     <row r="8" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D8" s="1" t="s">
@@ -790,19 +796,19 @@
         <v>11</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L8" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8" t="s">
+      <c r="L8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4" t="s">
         <v>0</v>
       </c>
     </row>
@@ -817,17 +823,17 @@
       <c r="H9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>17</v>
+      <c r="I9" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N9" s="2" t="s">
         <v>2</v>
@@ -839,138 +845,138 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
+      <c r="H11" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
       <c r="L11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H12" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8" t="s">
+      <c r="H12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="D13" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
       <c r="H13" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D14" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8" t="s">
+      <c r="D14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>17</v>
+      <c r="I14" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
+      <c r="L14" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
     </row>
     <row r="15" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D15" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="J15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L15" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8" t="s">
+      <c r="L15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>17</v>
+        <v>34</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>2</v>
@@ -978,14 +984,14 @@
     </row>
     <row r="17" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E17" s="1"/>
-      <c r="F17" s="1" t="s">
-        <v>12</v>
+      <c r="F17" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M17" s="1"/>
       <c r="N17" s="1" t="s">
@@ -994,33 +1000,33 @@
     </row>
     <row r="18" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D18" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E18" s="1"/>
-      <c r="F18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
+      <c r="F18" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
     </row>
     <row r="19" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H19" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8" t="s">
+      <c r="H19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1028,72 +1034,72 @@
       <c r="D20" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>17</v>
+      <c r="E20" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L20" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
+      <c r="L20" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
     </row>
     <row r="21" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D21" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L21" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8" t="s">
+      <c r="L21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N22" s="2" t="s">
         <v>2</v>
@@ -1101,14 +1107,14 @@
     </row>
     <row r="23" spans="4:14" x14ac:dyDescent="0.3">
       <c r="H23" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M23" s="1"/>
       <c r="N23" s="1" t="s">
@@ -1117,19 +1123,19 @@
     </row>
     <row r="24" spans="4:14" x14ac:dyDescent="0.3">
       <c r="H24" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I24" s="1"/>
       <c r="J24" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="4:14" x14ac:dyDescent="0.3">
       <c r="H25" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>2</v>
@@ -1137,15 +1143,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="H11:J11"/>
     <mergeCell ref="H18:J18"/>
     <mergeCell ref="L2:N2"/>
     <mergeCell ref="L7:N7"/>
     <mergeCell ref="L14:N14"/>
     <mergeCell ref="L20:N20"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="H11:J11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>